<commit_message>
Files updated to run with Extent Reports
</commit_message>
<xml_diff>
--- a/src/test/resources/prac/mda/excel/testData.xlsx
+++ b/src/test/resources/prac/mda/excel/testData.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mayuresh\Learning\Programming\Java\Workspace\PageObjectModel_MDA\src\test\resources\prac\mda\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mayuresh\Learning\Programming\Java\Workspace\POM_PageFactories\src\test\resources\prac\mda\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33677F02-451C-4957-9123-454819D79256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061596B9-C740-4449-9C98-C46E59AE3159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7EE84A7D-FAAE-449B-A0DD-85079EA1ADA3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{7EE84A7D-FAAE-449B-A0DD-85079EA1ADA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Suite" sheetId="3" r:id="rId1"/>
     <sheet name="LoginTest" sheetId="4" r:id="rId2"/>
-    <sheet name="CreateAccountTest" sheetId="5" r:id="rId3"/>
+    <sheet name="SearchTest" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -53,9 +53,6 @@
     <t>Pratapgad10November</t>
   </si>
   <si>
-    <t>CreateAccountTest</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
@@ -63,6 +60,9 @@
   </si>
   <si>
     <t>Ahirrao</t>
+  </si>
+  <si>
+    <t>SearchTest</t>
   </si>
 </sst>
 </file>
@@ -416,7 +416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B00325D4-AA8A-4C05-9C19-B9A9DC4E33EB}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -444,10 +444,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15523A9C-E384-4C7C-A98B-D61657FEE69E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -512,7 +512,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -520,7 +520,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Latest code commit: 2 Jan 2022
</commit_message>
<xml_diff>
--- a/src/test/resources/prac/mda/excel/testData.xlsx
+++ b/src/test/resources/prac/mda/excel/testData.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mayuresh\Learning\Programming\Java\Workspace\POM_PageFactories\src\test\resources\prac\mda\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061596B9-C740-4449-9C98-C46E59AE3159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{7EE84A7D-FAAE-449B-A0DD-85079EA1ADA3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Suite" sheetId="3" r:id="rId1"/>
     <sheet name="LoginTest" sheetId="4" r:id="rId2"/>
     <sheet name="SearchTest" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>RunMode</t>
   </si>
@@ -47,28 +46,34 @@
     <t>Password</t>
   </si>
   <si>
-    <t>md.ahirrao@gmail.com</t>
-  </si>
-  <si>
-    <t>Pratapgad10November</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
-    <t>AccountName</t>
-  </si>
-  <si>
-    <t>Ahirrao</t>
-  </si>
-  <si>
     <t>SearchTest</t>
+  </si>
+  <si>
+    <t>Automation Testing</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>mayuresh.ahirrao@gmail.com</t>
+  </si>
+  <si>
+    <t>Mayur31885</t>
+  </si>
+  <si>
+    <t>SearchKey</t>
+  </si>
+  <si>
+    <t>Location</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -413,7 +418,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B00325D4-AA8A-4C05-9C19-B9A9DC4E33EB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -444,10 +449,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -457,11 +462,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88FE4727-84F3-4152-8556-B5C952B3245F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -483,10 +488,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -498,31 +503,38 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15523A9C-E384-4C7C-A98B-D61657FEE69E}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>